<commit_message>
fixed NA problems, there is no unemployment data for asian before 2003, so changed the time range from 2000-2020 to 2003-2020. Fixed it in all source excel files, and .RData is readioly usable
</commit_message>
<xml_diff>
--- a/data/Labor Force Statistics from the Current Population Survey, 40 matrixes/Unemployment Rate - 16-19 Years - LNS14000012.xlsx
+++ b/data/Labor Force Statistics from the Current Population Survey, 40 matrixes/Unemployment Rate - 16-19 Years - LNS14000012.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ziyuan/Desktop/info_201/mango-mochi-project/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ziyuan/Desktop/info_201/mango-mochi-project/data/Labor Force Statistics from the Current Population Survey, 40 matrixes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DA3D08D-BCC3-7B46-86BD-A9A7B43A4941}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAE8EAB3-6063-BB4B-B367-1A838D6C8282}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -112,7 +112,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="#0.0"/>
+    <numFmt numFmtId="164" formatCode="#0.0"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -204,24 +204,24 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -537,11 +537,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M22"/>
+  <dimension ref="A1:M19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:XFD11"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -593,853 +593,730 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
-        <v>2000</v>
+        <v>2003</v>
       </c>
       <c r="B2" s="3">
-        <v>12.7</v>
+        <v>17.2</v>
       </c>
       <c r="C2" s="3">
-        <v>13.8</v>
+        <v>17.2</v>
       </c>
       <c r="D2" s="3">
-        <v>13.3</v>
+        <v>17.8</v>
       </c>
       <c r="E2" s="3">
-        <v>12.6</v>
+        <v>17.7</v>
       </c>
       <c r="F2" s="3">
-        <v>12.8</v>
+        <v>17.899999999999999</v>
       </c>
       <c r="G2" s="3">
-        <v>12.3</v>
+        <v>19</v>
       </c>
       <c r="H2" s="3">
-        <v>13.4</v>
+        <v>18.2</v>
       </c>
       <c r="I2" s="3">
-        <v>14</v>
+        <v>16.600000000000001</v>
       </c>
       <c r="J2" s="3">
-        <v>13</v>
+        <v>17.600000000000001</v>
       </c>
       <c r="K2" s="3">
-        <v>12.8</v>
+        <v>17.2</v>
       </c>
       <c r="L2" s="3">
-        <v>13</v>
+        <v>15.7</v>
       </c>
       <c r="M2" s="3">
-        <v>13.2</v>
+        <v>16.2</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
-        <v>2001</v>
+        <v>2004</v>
       </c>
       <c r="B3" s="3">
-        <v>13.8</v>
+        <v>17</v>
       </c>
       <c r="C3" s="3">
-        <v>13.7</v>
+        <v>16.5</v>
       </c>
       <c r="D3" s="3">
-        <v>13.8</v>
+        <v>16.8</v>
       </c>
       <c r="E3" s="3">
-        <v>13.9</v>
+        <v>16.600000000000001</v>
       </c>
       <c r="F3" s="3">
-        <v>13.4</v>
+        <v>17.100000000000001</v>
       </c>
       <c r="G3" s="3">
-        <v>14.2</v>
+        <v>17</v>
       </c>
       <c r="H3" s="3">
-        <v>14.4</v>
+        <v>17.8</v>
       </c>
       <c r="I3" s="3">
-        <v>15.6</v>
+        <v>16.7</v>
       </c>
       <c r="J3" s="3">
-        <v>15.2</v>
+        <v>16.600000000000001</v>
       </c>
       <c r="K3" s="3">
-        <v>16</v>
+        <v>17.399999999999999</v>
       </c>
       <c r="L3" s="3">
-        <v>15.9</v>
+        <v>16.399999999999999</v>
       </c>
       <c r="M3" s="3">
-        <v>17</v>
+        <v>17.600000000000001</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
-        <v>2002</v>
+        <v>2005</v>
       </c>
       <c r="B4" s="3">
-        <v>16.5</v>
+        <v>16.2</v>
       </c>
       <c r="C4" s="3">
-        <v>16</v>
+        <v>17.5</v>
       </c>
       <c r="D4" s="3">
-        <v>16.600000000000001</v>
+        <v>17.100000000000001</v>
       </c>
       <c r="E4" s="3">
-        <v>16.7</v>
+        <v>17.8</v>
       </c>
       <c r="F4" s="3">
-        <v>16.600000000000001</v>
+        <v>17.8</v>
       </c>
       <c r="G4" s="3">
-        <v>16.7</v>
+        <v>16.3</v>
       </c>
       <c r="H4" s="3">
-        <v>16.8</v>
+        <v>16.100000000000001</v>
       </c>
       <c r="I4" s="3">
+        <v>16.100000000000001</v>
+      </c>
+      <c r="J4" s="3">
+        <v>15.5</v>
+      </c>
+      <c r="K4" s="3">
+        <v>16.100000000000001</v>
+      </c>
+      <c r="L4" s="3">
         <v>17</v>
       </c>
-      <c r="J4" s="3">
-        <v>16.3</v>
-      </c>
-      <c r="K4" s="3">
-        <v>15.1</v>
-      </c>
-      <c r="L4" s="3">
-        <v>17.100000000000001</v>
-      </c>
       <c r="M4" s="3">
-        <v>16.899999999999999</v>
+        <v>14.9</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
-        <v>2003</v>
+        <v>2006</v>
       </c>
       <c r="B5" s="3">
-        <v>17.2</v>
+        <v>15.1</v>
       </c>
       <c r="C5" s="3">
-        <v>17.2</v>
+        <v>15.3</v>
       </c>
       <c r="D5" s="3">
-        <v>17.8</v>
+        <v>16.100000000000001</v>
       </c>
       <c r="E5" s="3">
-        <v>17.7</v>
+        <v>14.6</v>
       </c>
       <c r="F5" s="3">
-        <v>17.899999999999999</v>
+        <v>14</v>
       </c>
       <c r="G5" s="3">
-        <v>19</v>
+        <v>15.8</v>
       </c>
       <c r="H5" s="3">
-        <v>18.2</v>
+        <v>15.9</v>
       </c>
       <c r="I5" s="3">
-        <v>16.600000000000001</v>
+        <v>16</v>
       </c>
       <c r="J5" s="3">
-        <v>17.600000000000001</v>
+        <v>16.3</v>
       </c>
       <c r="K5" s="3">
-        <v>17.2</v>
+        <v>15.2</v>
       </c>
       <c r="L5" s="3">
-        <v>15.7</v>
+        <v>14.8</v>
       </c>
       <c r="M5" s="3">
-        <v>16.2</v>
+        <v>14.6</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
-        <v>2004</v>
+        <v>2007</v>
       </c>
       <c r="B6" s="3">
-        <v>17</v>
+        <v>14.8</v>
       </c>
       <c r="C6" s="3">
-        <v>16.5</v>
+        <v>14.9</v>
       </c>
       <c r="D6" s="3">
+        <v>14.9</v>
+      </c>
+      <c r="E6" s="3">
+        <v>15.9</v>
+      </c>
+      <c r="F6" s="3">
+        <v>15.9</v>
+      </c>
+      <c r="G6" s="3">
+        <v>16.3</v>
+      </c>
+      <c r="H6" s="3">
+        <v>15.3</v>
+      </c>
+      <c r="I6" s="3">
+        <v>15.9</v>
+      </c>
+      <c r="J6" s="3">
+        <v>15.9</v>
+      </c>
+      <c r="K6" s="3">
+        <v>15.4</v>
+      </c>
+      <c r="L6" s="3">
+        <v>16.2</v>
+      </c>
+      <c r="M6" s="3">
         <v>16.8</v>
-      </c>
-      <c r="E6" s="3">
-        <v>16.600000000000001</v>
-      </c>
-      <c r="F6" s="3">
-        <v>17.100000000000001</v>
-      </c>
-      <c r="G6" s="3">
-        <v>17</v>
-      </c>
-      <c r="H6" s="3">
-        <v>17.8</v>
-      </c>
-      <c r="I6" s="3">
-        <v>16.7</v>
-      </c>
-      <c r="J6" s="3">
-        <v>16.600000000000001</v>
-      </c>
-      <c r="K6" s="3">
-        <v>17.399999999999999</v>
-      </c>
-      <c r="L6" s="3">
-        <v>16.399999999999999</v>
-      </c>
-      <c r="M6" s="3">
-        <v>17.600000000000001</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
-        <v>2005</v>
+        <v>2008</v>
       </c>
       <c r="B7" s="3">
-        <v>16.2</v>
+        <v>17.8</v>
       </c>
       <c r="C7" s="3">
-        <v>17.5</v>
+        <v>16.600000000000001</v>
       </c>
       <c r="D7" s="3">
-        <v>17.100000000000001</v>
+        <v>16.100000000000001</v>
       </c>
       <c r="E7" s="3">
-        <v>17.8</v>
+        <v>15.9</v>
       </c>
       <c r="F7" s="3">
-        <v>17.8</v>
+        <v>19</v>
       </c>
       <c r="G7" s="3">
-        <v>16.3</v>
+        <v>19.2</v>
       </c>
       <c r="H7" s="3">
-        <v>16.100000000000001</v>
+        <v>20.7</v>
       </c>
       <c r="I7" s="3">
-        <v>16.100000000000001</v>
+        <v>18.600000000000001</v>
       </c>
       <c r="J7" s="3">
-        <v>15.5</v>
+        <v>19.100000000000001</v>
       </c>
       <c r="K7" s="3">
-        <v>16.100000000000001</v>
+        <v>20</v>
       </c>
       <c r="L7" s="3">
-        <v>17</v>
+        <v>20.3</v>
       </c>
       <c r="M7" s="3">
-        <v>14.9</v>
+        <v>20.5</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
-        <v>2006</v>
+        <v>2009</v>
       </c>
       <c r="B8" s="3">
-        <v>15.1</v>
+        <v>20.7</v>
       </c>
       <c r="C8" s="3">
-        <v>15.3</v>
+        <v>22.3</v>
       </c>
       <c r="D8" s="3">
-        <v>16.100000000000001</v>
+        <v>22.2</v>
       </c>
       <c r="E8" s="3">
-        <v>14.6</v>
+        <v>22.2</v>
       </c>
       <c r="F8" s="3">
-        <v>14</v>
+        <v>23.4</v>
       </c>
       <c r="G8" s="3">
-        <v>15.8</v>
+        <v>24.7</v>
       </c>
       <c r="H8" s="3">
-        <v>15.9</v>
+        <v>24.3</v>
       </c>
       <c r="I8" s="3">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="J8" s="3">
-        <v>16.3</v>
+        <v>25.9</v>
       </c>
       <c r="K8" s="3">
-        <v>15.2</v>
+        <v>27.2</v>
       </c>
       <c r="L8" s="3">
-        <v>14.8</v>
+        <v>26.9</v>
       </c>
       <c r="M8" s="3">
-        <v>14.6</v>
+        <v>26.7</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
-        <v>2007</v>
+        <v>2010</v>
       </c>
       <c r="B9" s="3">
-        <v>14.8</v>
+        <v>26.1</v>
       </c>
       <c r="C9" s="3">
-        <v>14.9</v>
+        <v>25.6</v>
       </c>
       <c r="D9" s="3">
-        <v>14.9</v>
+        <v>26.2</v>
       </c>
       <c r="E9" s="3">
-        <v>15.9</v>
+        <v>25.4</v>
       </c>
       <c r="F9" s="3">
-        <v>15.9</v>
+        <v>26.5</v>
       </c>
       <c r="G9" s="3">
-        <v>16.3</v>
+        <v>25.9</v>
       </c>
       <c r="H9" s="3">
-        <v>15.3</v>
+        <v>25.9</v>
       </c>
       <c r="I9" s="3">
-        <v>15.9</v>
+        <v>25.5</v>
       </c>
       <c r="J9" s="3">
-        <v>15.9</v>
+        <v>25.8</v>
       </c>
       <c r="K9" s="3">
-        <v>15.4</v>
+        <v>27.2</v>
       </c>
       <c r="L9" s="3">
-        <v>16.2</v>
+        <v>24.8</v>
       </c>
       <c r="M9" s="3">
-        <v>16.8</v>
+        <v>25.3</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
-        <v>2008</v>
+        <v>2011</v>
       </c>
       <c r="B10" s="3">
-        <v>17.8</v>
+        <v>25.7</v>
       </c>
       <c r="C10" s="3">
-        <v>16.600000000000001</v>
+        <v>24.1</v>
       </c>
       <c r="D10" s="3">
-        <v>16.100000000000001</v>
+        <v>24.4</v>
       </c>
       <c r="E10" s="3">
-        <v>15.9</v>
+        <v>24.7</v>
       </c>
       <c r="F10" s="3">
-        <v>19</v>
+        <v>23.9</v>
       </c>
       <c r="G10" s="3">
-        <v>19.2</v>
+        <v>24.5</v>
       </c>
       <c r="H10" s="3">
-        <v>20.7</v>
+        <v>24.7</v>
       </c>
       <c r="I10" s="3">
-        <v>18.600000000000001</v>
+        <v>25</v>
       </c>
       <c r="J10" s="3">
-        <v>19.100000000000001</v>
+        <v>24.4</v>
       </c>
       <c r="K10" s="3">
-        <v>20</v>
+        <v>24.2</v>
       </c>
       <c r="L10" s="3">
-        <v>20.3</v>
+        <v>24.2</v>
       </c>
       <c r="M10" s="3">
-        <v>20.5</v>
+        <v>23.3</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
-        <v>2009</v>
+        <v>2012</v>
       </c>
       <c r="B11" s="3">
-        <v>20.7</v>
+        <v>23.6</v>
       </c>
       <c r="C11" s="3">
-        <v>22.3</v>
+        <v>23.8</v>
       </c>
       <c r="D11" s="3">
-        <v>22.2</v>
+        <v>24.8</v>
       </c>
       <c r="E11" s="3">
-        <v>22.2</v>
+        <v>25</v>
       </c>
       <c r="F11" s="3">
-        <v>23.4</v>
+        <v>24.4</v>
       </c>
       <c r="G11" s="3">
-        <v>24.7</v>
+        <v>23.3</v>
       </c>
       <c r="H11" s="3">
-        <v>24.3</v>
+        <v>23.6</v>
       </c>
       <c r="I11" s="3">
-        <v>25</v>
+        <v>24.2</v>
       </c>
       <c r="J11" s="3">
-        <v>25.9</v>
+        <v>23.8</v>
       </c>
       <c r="K11" s="3">
-        <v>27.2</v>
+        <v>23.9</v>
       </c>
       <c r="L11" s="3">
-        <v>26.9</v>
+        <v>23.9</v>
       </c>
       <c r="M11" s="3">
-        <v>26.7</v>
+        <v>24.1</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
-        <v>2010</v>
+        <v>2013</v>
       </c>
       <c r="B12" s="3">
-        <v>26.1</v>
+        <v>23.7</v>
       </c>
       <c r="C12" s="3">
-        <v>25.6</v>
+        <v>25.2</v>
       </c>
       <c r="D12" s="3">
-        <v>26.2</v>
+        <v>24</v>
       </c>
       <c r="E12" s="3">
-        <v>25.4</v>
+        <v>24.4</v>
       </c>
       <c r="F12" s="3">
-        <v>26.5</v>
+        <v>24.4</v>
       </c>
       <c r="G12" s="3">
-        <v>25.9</v>
+        <v>23.1</v>
       </c>
       <c r="H12" s="3">
-        <v>25.9</v>
+        <v>23.3</v>
       </c>
       <c r="I12" s="3">
-        <v>25.5</v>
+        <v>22.5</v>
       </c>
       <c r="J12" s="3">
-        <v>25.8</v>
+        <v>21.3</v>
       </c>
       <c r="K12" s="3">
-        <v>27.2</v>
+        <v>22.2</v>
       </c>
       <c r="L12" s="3">
-        <v>24.8</v>
+        <v>20.7</v>
       </c>
       <c r="M12" s="3">
-        <v>25.3</v>
+        <v>20.399999999999999</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
-        <v>2011</v>
+        <v>2014</v>
       </c>
       <c r="B13" s="3">
-        <v>25.7</v>
+        <v>20.399999999999999</v>
       </c>
       <c r="C13" s="3">
-        <v>24.1</v>
+        <v>21.4</v>
       </c>
       <c r="D13" s="3">
-        <v>24.4</v>
+        <v>20.8</v>
       </c>
       <c r="E13" s="3">
-        <v>24.7</v>
+        <v>19.399999999999999</v>
       </c>
       <c r="F13" s="3">
-        <v>23.9</v>
+        <v>19.3</v>
       </c>
       <c r="G13" s="3">
-        <v>24.5</v>
+        <v>20.399999999999999</v>
       </c>
       <c r="H13" s="3">
-        <v>24.7</v>
+        <v>20.3</v>
       </c>
       <c r="I13" s="3">
-        <v>25</v>
+        <v>19.399999999999999</v>
       </c>
       <c r="J13" s="3">
-        <v>24.4</v>
+        <v>20.100000000000001</v>
       </c>
       <c r="K13" s="3">
-        <v>24.2</v>
+        <v>18.7</v>
       </c>
       <c r="L13" s="3">
-        <v>24.2</v>
+        <v>17.2</v>
       </c>
       <c r="M13" s="3">
-        <v>23.3</v>
+        <v>16.899999999999999</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
-        <v>2012</v>
+        <v>2015</v>
       </c>
       <c r="B14" s="3">
-        <v>23.6</v>
+        <v>18.5</v>
       </c>
       <c r="C14" s="3">
-        <v>23.8</v>
+        <v>16.899999999999999</v>
       </c>
       <c r="D14" s="3">
-        <v>24.8</v>
+        <v>17.5</v>
       </c>
       <c r="E14" s="3">
-        <v>25</v>
+        <v>17.2</v>
       </c>
       <c r="F14" s="3">
-        <v>24.4</v>
+        <v>17.8</v>
       </c>
       <c r="G14" s="3">
-        <v>23.3</v>
+        <v>18</v>
       </c>
       <c r="H14" s="3">
-        <v>23.6</v>
+        <v>16.399999999999999</v>
       </c>
       <c r="I14" s="3">
-        <v>24.2</v>
+        <v>16.899999999999999</v>
       </c>
       <c r="J14" s="3">
-        <v>23.8</v>
+        <v>16.5</v>
       </c>
       <c r="K14" s="3">
-        <v>23.9</v>
+        <v>15.9</v>
       </c>
       <c r="L14" s="3">
-        <v>23.9</v>
+        <v>15.3</v>
       </c>
       <c r="M14" s="3">
-        <v>24.1</v>
+        <v>16.2</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
-        <v>2013</v>
+        <v>2016</v>
       </c>
       <c r="B15" s="3">
-        <v>23.7</v>
+        <v>15.7</v>
       </c>
       <c r="C15" s="3">
-        <v>25.2</v>
+        <v>15.2</v>
       </c>
       <c r="D15" s="3">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="E15" s="3">
-        <v>24.4</v>
+        <v>16</v>
       </c>
       <c r="F15" s="3">
-        <v>24.4</v>
+        <v>16</v>
       </c>
       <c r="G15" s="3">
-        <v>23.1</v>
+        <v>16.100000000000001</v>
       </c>
       <c r="H15" s="3">
-        <v>23.3</v>
+        <v>15.8</v>
       </c>
       <c r="I15" s="3">
-        <v>22.5</v>
+        <v>15.9</v>
       </c>
       <c r="J15" s="3">
-        <v>21.3</v>
+        <v>16.2</v>
       </c>
       <c r="K15" s="3">
-        <v>22.2</v>
+        <v>15.8</v>
       </c>
       <c r="L15" s="3">
-        <v>20.7</v>
+        <v>14.9</v>
       </c>
       <c r="M15" s="3">
-        <v>20.399999999999999</v>
+        <v>14.5</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
-        <v>2014</v>
+        <v>2017</v>
       </c>
       <c r="B16" s="3">
-        <v>20.399999999999999</v>
+        <v>14.6</v>
       </c>
       <c r="C16" s="3">
-        <v>21.4</v>
+        <v>14.4</v>
       </c>
       <c r="D16" s="3">
-        <v>20.8</v>
+        <v>13.7</v>
       </c>
       <c r="E16" s="3">
-        <v>19.399999999999999</v>
+        <v>14.7</v>
       </c>
       <c r="F16" s="3">
-        <v>19.3</v>
+        <v>14.1</v>
       </c>
       <c r="G16" s="3">
-        <v>20.399999999999999</v>
+        <v>13.4</v>
       </c>
       <c r="H16" s="3">
-        <v>20.3</v>
+        <v>13.2</v>
       </c>
       <c r="I16" s="3">
-        <v>19.399999999999999</v>
+        <v>13.9</v>
       </c>
       <c r="J16" s="3">
-        <v>20.100000000000001</v>
+        <v>13.1</v>
       </c>
       <c r="K16" s="3">
-        <v>18.7</v>
+        <v>14</v>
       </c>
       <c r="L16" s="3">
-        <v>17.2</v>
+        <v>16.100000000000001</v>
       </c>
       <c r="M16" s="3">
-        <v>16.899999999999999</v>
+        <v>13.7</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
-        <v>2015</v>
+        <v>2018</v>
       </c>
       <c r="B17" s="3">
-        <v>18.5</v>
+        <v>13.7</v>
       </c>
       <c r="C17" s="3">
-        <v>16.899999999999999</v>
+        <v>14</v>
       </c>
       <c r="D17" s="3">
-        <v>17.5</v>
+        <v>13.4</v>
       </c>
       <c r="E17" s="3">
-        <v>17.2</v>
+        <v>12.8</v>
       </c>
       <c r="F17" s="3">
-        <v>17.8</v>
+        <v>12.8</v>
       </c>
       <c r="G17" s="3">
-        <v>18</v>
+        <v>12.6</v>
       </c>
       <c r="H17" s="3">
-        <v>16.399999999999999</v>
+        <v>13</v>
       </c>
       <c r="I17" s="3">
-        <v>16.899999999999999</v>
+        <v>12.8</v>
       </c>
       <c r="J17" s="3">
-        <v>16.5</v>
+        <v>12.7</v>
       </c>
       <c r="K17" s="3">
-        <v>15.9</v>
+        <v>12.2</v>
       </c>
       <c r="L17" s="3">
-        <v>15.3</v>
+        <v>12.4</v>
       </c>
       <c r="M17" s="3">
-        <v>16.2</v>
+        <v>12.6</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
-        <v>2016</v>
+        <v>2019</v>
       </c>
       <c r="B18" s="3">
-        <v>15.7</v>
+        <v>12.9</v>
       </c>
       <c r="C18" s="3">
-        <v>15.2</v>
+        <v>13.3</v>
       </c>
       <c r="D18" s="3">
-        <v>16</v>
+        <v>12.7</v>
       </c>
       <c r="E18" s="3">
-        <v>16</v>
+        <v>12.9</v>
       </c>
       <c r="F18" s="3">
-        <v>16</v>
+        <v>12.6</v>
       </c>
       <c r="G18" s="3">
-        <v>16.100000000000001</v>
+        <v>12.7</v>
       </c>
       <c r="H18" s="3">
-        <v>15.8</v>
+        <v>12.7</v>
       </c>
       <c r="I18" s="3">
-        <v>15.9</v>
+        <v>12.5</v>
       </c>
       <c r="J18" s="3">
-        <v>16.2</v>
+        <v>12.5</v>
       </c>
       <c r="K18" s="3">
-        <v>15.8</v>
+        <v>12.3</v>
       </c>
       <c r="L18" s="3">
-        <v>14.9</v>
+        <v>12</v>
       </c>
       <c r="M18" s="3">
-        <v>14.5</v>
+        <v>12.6</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
-        <v>2017</v>
+        <v>2020</v>
       </c>
       <c r="B19" s="3">
-        <v>14.6</v>
+        <v>12.2</v>
       </c>
       <c r="C19" s="3">
-        <v>14.4</v>
+        <v>11</v>
       </c>
       <c r="D19" s="3">
-        <v>13.7</v>
+        <v>14.3</v>
       </c>
       <c r="E19" s="3">
-        <v>14.7</v>
+        <v>31.9</v>
       </c>
       <c r="F19" s="3">
-        <v>14.1</v>
+        <v>29.9</v>
       </c>
       <c r="G19" s="3">
-        <v>13.4</v>
+        <v>23.2</v>
       </c>
       <c r="H19" s="3">
-        <v>13.2</v>
+        <v>19.3</v>
       </c>
       <c r="I19" s="3">
-        <v>13.9</v>
+        <v>16.100000000000001</v>
       </c>
       <c r="J19" s="3">
-        <v>13.1</v>
-      </c>
-      <c r="K19" s="3">
-        <v>14</v>
-      </c>
-      <c r="L19" s="3">
-        <v>16.100000000000001</v>
-      </c>
-      <c r="M19" s="3">
-        <v>13.7</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A20" s="2">
-        <v>2018</v>
-      </c>
-      <c r="B20" s="3">
-        <v>13.7</v>
-      </c>
-      <c r="C20" s="3">
-        <v>14</v>
-      </c>
-      <c r="D20" s="3">
-        <v>13.4</v>
-      </c>
-      <c r="E20" s="3">
-        <v>12.8</v>
-      </c>
-      <c r="F20" s="3">
-        <v>12.8</v>
-      </c>
-      <c r="G20" s="3">
-        <v>12.6</v>
-      </c>
-      <c r="H20" s="3">
-        <v>13</v>
-      </c>
-      <c r="I20" s="3">
-        <v>12.8</v>
-      </c>
-      <c r="J20" s="3">
-        <v>12.7</v>
-      </c>
-      <c r="K20" s="3">
-        <v>12.2</v>
-      </c>
-      <c r="L20" s="3">
-        <v>12.4</v>
-      </c>
-      <c r="M20" s="3">
-        <v>12.6</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A21" s="2">
-        <v>2019</v>
-      </c>
-      <c r="B21" s="3">
-        <v>12.9</v>
-      </c>
-      <c r="C21" s="3">
-        <v>13.3</v>
-      </c>
-      <c r="D21" s="3">
-        <v>12.7</v>
-      </c>
-      <c r="E21" s="3">
-        <v>12.9</v>
-      </c>
-      <c r="F21" s="3">
-        <v>12.6</v>
-      </c>
-      <c r="G21" s="3">
-        <v>12.7</v>
-      </c>
-      <c r="H21" s="3">
-        <v>12.7</v>
-      </c>
-      <c r="I21" s="3">
-        <v>12.5</v>
-      </c>
-      <c r="J21" s="3">
-        <v>12.5</v>
-      </c>
-      <c r="K21" s="3">
-        <v>12.3</v>
-      </c>
-      <c r="L21" s="3">
-        <v>12</v>
-      </c>
-      <c r="M21" s="3">
-        <v>12.6</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A22" s="2">
-        <v>2020</v>
-      </c>
-      <c r="B22" s="3">
-        <v>12.2</v>
-      </c>
-      <c r="C22" s="3">
-        <v>11</v>
-      </c>
-      <c r="D22" s="3">
-        <v>14.3</v>
-      </c>
-      <c r="E22" s="3">
-        <v>31.9</v>
-      </c>
-      <c r="F22" s="3">
-        <v>29.9</v>
-      </c>
-      <c r="G22" s="3">
-        <v>23.2</v>
-      </c>
-      <c r="H22" s="3">
-        <v>19.3</v>
-      </c>
-      <c r="I22" s="3">
-        <v>16.100000000000001</v>
-      </c>
-      <c r="J22" s="3">
         <v>15.9</v>
       </c>
     </row>
@@ -1464,7 +1341,7 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="6"/>
@@ -1474,7 +1351,7 @@
       <c r="F1" s="6"/>
     </row>
     <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="6"/>
@@ -1495,7 +1372,7 @@
       <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="6"/>
@@ -1504,7 +1381,7 @@
       <c r="F4" s="6"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="9" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="6"/>
@@ -1517,7 +1394,7 @@
       <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C6" s="6"/>
@@ -1525,11 +1402,11 @@
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" ht="28" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C7" s="6"/>
@@ -1537,11 +1414,11 @@
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" ht="28" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="5" t="s">
         <v>10</v>
       </c>
       <c r="C8" s="6"/>
@@ -1553,7 +1430,7 @@
       <c r="A9" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C9" s="6"/>
@@ -1565,7 +1442,7 @@
       <c r="A10" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="7" t="s">
         <v>14</v>
       </c>
       <c r="C10" s="6"/>

</xml_diff>